<commit_message>
Fixed some formulas on template.xlsx
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguecor/python/ndo_epg_migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45966DBE-846E-8B46-AB07-C806DF835848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D5BEFA-354C-024C-A36D-3BCFADEA70CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="49980" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="49980" windowHeight="28300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Infra" sheetId="1" r:id="rId1"/>
@@ -378,7 +378,7 @@
     <t>Dest EPG Name</t>
   </si>
   <si>
-    <t>Consumed Contract</t>
+    <t>Consumed Contract Reference</t>
   </si>
 </sst>
 </file>
@@ -19003,7 +19003,7 @@
   </sheetPr>
   <dimension ref="A2:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:O15"/>
     </sheetView>
   </sheetViews>
@@ -19762,8 +19762,8 @@
   </sheetPr>
   <dimension ref="A1:AE389"/>
   <sheetViews>
-    <sheetView topLeftCell="D63" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+    <sheetView tabSelected="1" topLeftCell="M291" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="P303" sqref="P303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19785,7 +19785,7 @@
     <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.6640625" customWidth="1"/>
     <col min="27" max="27" width="22.5" customWidth="1"/>
     <col min="28" max="29" width="19.1640625" customWidth="1"/>
   </cols>
@@ -22921,7 +22921,7 @@
         <v/>
       </c>
       <c r="AE303" s="53" t="str">
-        <f>IF($AA303="","",INDEX(AB55:AB298,MATCH(AC303,AC55:AC298,0),1))</f>
+        <f>IF($AA303="","",INDEX($AB$55:$AB$298,MATCH(AC303,$AC$55:$AC$298,0),1))</f>
         <v/>
       </c>
     </row>
@@ -23029,7 +23029,7 @@
         <v/>
       </c>
       <c r="AE304" s="58" t="str">
-        <f>IF($AA304="","",INDEX(AB56:AB299,MATCH(AC304,AC56:AC299,0),1))</f>
+        <f t="shared" ref="AE304:AE343" si="22">IF($AA304="","",INDEX($AB$55:$AB$298,MATCH(AC304,$AC$55:$AC$298,0),1))</f>
         <v/>
       </c>
     </row>
@@ -23137,7 +23137,7 @@
         <v/>
       </c>
       <c r="AE305" s="63" t="str">
-        <f t="shared" ref="AE305:AE343" si="22">IF($AA305="","",INDEX(AB57:AB301,MATCH(AC305,AC57:AC301,0),1))</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>

</xml_diff>